<commit_message>
New Selenium 4.2 Updated without WebDriver Manager
</commit_message>
<xml_diff>
--- a/src/test/java/com/inetBanking/testData/CustomerDetails.xlsx
+++ b/src/test/java/com/inetBanking/testData/CustomerDetails.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="79">
   <si>
     <t>Customer ID</t>
   </si>
@@ -245,6 +245,12 @@
   </si>
   <si>
     <t>iDpKkPSV@gmail.com</t>
+  </si>
+  <si>
+    <t>26172</t>
+  </si>
+  <si>
+    <t>EWqlpZyQ@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -662,7 +668,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -689,7 +695,7 @@
         <v>18</v>
       </c>
       <c r="J2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>